<commit_message>
Added section number and csid to faculty model, changed appropiate methods and views.
</commit_message>
<xml_diff>
--- a/data/facultyTemp.xlsx
+++ b/data/facultyTemp.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -399,209 +399,1054 @@
       <c r="F1" t="str">
         <v>admin</v>
       </c>
+      <c r="G1" t="str">
+        <v>csID</v>
+      </c>
+      <c r="H1" t="str">
+        <v>sectionNumber</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Svflann</v>
+        <v>ahalt</v>
       </c>
       <c r="B2" t="str">
-        <v>Shane</v>
+        <v>Stanley</v>
       </c>
       <c r="C2" t="str">
-        <v>Flannigan</v>
+        <v>Ahalt</v>
       </c>
       <c r="D2">
-        <v>730015207</v>
+        <v>720046930</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
       </c>
       <c r="F2" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="G2" t="str">
+        <v>sdfasdf</v>
+      </c>
+      <c r="H2">
+        <v>33</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>jmajikes</v>
+        <v>aikat</v>
       </c>
       <c r="B3" t="str">
-        <v>John</v>
+        <v>Jay</v>
       </c>
       <c r="C3" t="str">
-        <v>Majikes</v>
+        <v>Aikat</v>
       </c>
       <c r="D3">
-        <v>123456789</v>
+        <v>704273269</v>
       </c>
       <c r="E3" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="str">
+        <v>the</v>
+      </c>
+      <c r="H3">
+        <v>234</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Dmanila</v>
+        <v>ron</v>
       </c>
       <c r="B4" t="str">
-        <v>Daniel</v>
+        <v>Ron</v>
       </c>
       <c r="C4" t="str">
-        <v>Manila</v>
+        <v>Alterovitz</v>
       </c>
       <c r="D4">
-        <v>730148808</v>
+        <v>714730206</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
       <c r="F4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>kmp</v>
+        <v>anderson</v>
       </c>
       <c r="B5" t="str">
-        <v>Ketan</v>
+        <v>Jim</v>
       </c>
       <c r="C5" t="str">
-        <v>Mayer-patel</v>
+        <v>Anderson</v>
       </c>
       <c r="D5">
-        <v>589302953</v>
+        <v>704290844</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>banana</v>
+        <v>Tasd</v>
       </c>
       <c r="B6" t="str">
-        <v>Mack</v>
+        <v>Tat</v>
       </c>
       <c r="C6" t="str">
-        <v>Monkey</v>
+        <v>Atat</v>
       </c>
       <c r="D6">
-        <v>123456788</v>
+        <v>324555334</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="str">
+        <v>Tasd</v>
+      </c>
+      <c r="H6">
+        <v>24</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>joliva</v>
+        <v>mbansal</v>
       </c>
       <c r="B7" t="str">
-        <v>Junier</v>
+        <v>Mohit</v>
       </c>
       <c r="C7" t="str">
-        <v>Oliva</v>
+        <v>Bansal</v>
       </c>
       <c r="D7">
-        <v>777777777</v>
+        <v>730139106</v>
       </c>
       <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>phelps</v>
+        <v>aberg</v>
       </c>
       <c r="B8" t="str">
-        <v>Michael</v>
+        <v>Alexander</v>
       </c>
       <c r="C8" t="str">
-        <v>Phelps</v>
+        <v>Berg</v>
       </c>
       <c r="D8">
-        <v>145244955</v>
+        <v>720450915</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Pozefsky</v>
+        <v>tlberg</v>
       </c>
       <c r="B9" t="str">
-        <v>Diane</v>
+        <v>Tamara</v>
       </c>
       <c r="C9" t="str">
-        <v>Pozefsky</v>
+        <v>Berg</v>
       </c>
       <c r="D9">
-        <v>701569707</v>
+        <v>720450914</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
       </c>
       <c r="F9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Takoda</v>
+        <v>gb</v>
       </c>
       <c r="B10" t="str">
-        <v>Takoda</v>
+        <v>Gary</v>
       </c>
       <c r="C10" t="str">
-        <v>Ren</v>
+        <v>Bishop</v>
       </c>
       <c r="D10">
-        <v>730093699</v>
+        <v>701876731</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
       </c>
       <c r="F10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>kris</v>
+        <v>dewan</v>
       </c>
       <c r="B11" t="str">
-        <v>kris</v>
+        <v>Prasun</v>
       </c>
       <c r="C11" t="str">
-        <v>jordan</v>
+        <v>Dewan</v>
       </c>
       <c r="D11">
-        <v>222222222</v>
+        <v>704279085</v>
       </c>
       <c r="E11" t="b">
         <v>1</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>js</v>
+        <v>psd</v>
       </c>
       <c r="B12" t="str">
-        <v>jack</v>
+        <v>Sridhar</v>
       </c>
       <c r="C12" t="str">
+        <v>Duggirala</v>
+      </c>
+      <c r="D12">
+        <v>730300195</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>dunn</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Enrique</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Dunn</v>
+      </c>
+      <c r="D13">
+        <v>714405371</v>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>fern</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Michael</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Fern</v>
+      </c>
+      <c r="D14">
+        <v>707772659</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Svflann</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Shane</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Flannigan</v>
+      </c>
+      <c r="D15">
+        <v>730015207</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>rjf</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Rob</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Fowler</v>
+      </c>
+      <c r="D16">
+        <v>713281075</v>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>jmf</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Jan-Michael</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Frahm</v>
+      </c>
+      <c r="D17">
+        <v>711856002</v>
+      </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>fuchs</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Henry</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Fuchs</v>
+      </c>
+      <c r="D18">
+        <v>704288472</v>
+      </c>
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>jeffay</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Kevin</v>
+      </c>
+      <c r="C19" t="str">
+        <v>Jeffay</v>
+      </c>
+      <c r="D19">
+        <v>704275348</v>
+      </c>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>kris</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Kris</v>
+      </c>
+      <c r="C20" t="str">
+        <v>Jordan</v>
+      </c>
+      <c r="D20">
+        <v>710453084</v>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>nicholas</v>
+      </c>
+      <c r="B21" t="str">
+        <v>Tessa</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Joseph-Nicholas</v>
+      </c>
+      <c r="D21">
+        <v>705472186</v>
+      </c>
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>jasleen</v>
+      </c>
+      <c r="B22" t="str">
+        <v>Jasleen</v>
+      </c>
+      <c r="C22" t="str">
+        <v>Kaur</v>
+      </c>
+      <c r="D22">
+        <v>710233624</v>
+      </c>
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+      <c r="F22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>ashokk</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Ashok</v>
+      </c>
+      <c r="C23" t="str">
+        <v>Krishnamurthy</v>
+      </c>
+      <c r="D23">
+        <v>720441075</v>
+      </c>
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>lin</v>
+      </c>
+      <c r="B24" t="str">
+        <v>Ming</v>
+      </c>
+      <c r="C24" t="str">
+        <v>Lin</v>
+      </c>
+      <c r="D24">
+        <v>704288661</v>
+      </c>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>jmajikes</v>
+      </c>
+      <c r="B25" t="str">
+        <v>John</v>
+      </c>
+      <c r="C25" t="str">
+        <v>Majikes</v>
+      </c>
+      <c r="D25">
+        <v>720176068</v>
+      </c>
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>dm</v>
+      </c>
+      <c r="B26" t="str">
+        <v>Dinesh</v>
+      </c>
+      <c r="C26" t="str">
+        <v>Manocha</v>
+      </c>
+      <c r="D26">
+        <v>704274598</v>
+      </c>
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
+      <c r="F26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>kmp</v>
+      </c>
+      <c r="B27" t="str">
+        <v>Ketan</v>
+      </c>
+      <c r="C27" t="str">
+        <v>Mayer-Patel</v>
+      </c>
+      <c r="D27">
+        <v>707696375</v>
+      </c>
+      <c r="E27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>mcmillan</v>
+      </c>
+      <c r="B28" t="str">
+        <v>Leonard</v>
+      </c>
+      <c r="C28" t="str">
+        <v>McMillan</v>
+      </c>
+      <c r="D28">
+        <v>703745132</v>
+      </c>
+      <c r="E28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>fabian</v>
+      </c>
+      <c r="B29" t="str">
+        <v>Fabian</v>
+      </c>
+      <c r="C29" t="str">
+        <v>Monrose</v>
+      </c>
+      <c r="D29">
+        <v>714634900</v>
+      </c>
+      <c r="E29" t="b">
+        <v>1</v>
+      </c>
+      <c r="F29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>mn</v>
+      </c>
+      <c r="B30" t="str">
+        <v>Marc</v>
+      </c>
+      <c r="C30" t="str">
+        <v>Niethammer</v>
+      </c>
+      <c r="D30">
+        <v>714077170</v>
+      </c>
+      <c r="E30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>nirjon</v>
+      </c>
+      <c r="B31" t="str">
+        <v>Shahriar</v>
+      </c>
+      <c r="C31" t="str">
+        <v>Nirjon</v>
+      </c>
+      <c r="D31">
+        <v>730064202</v>
+      </c>
+      <c r="E31" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>ipek</v>
+      </c>
+      <c r="B32" t="str">
+        <v>Ipek</v>
+      </c>
+      <c r="C32" t="str">
+        <v>Oguz</v>
+      </c>
+      <c r="D32">
+        <v>710990354</v>
+      </c>
+      <c r="E32" t="b">
+        <v>1</v>
+      </c>
+      <c r="F32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>joliva</v>
+      </c>
+      <c r="B33" t="str">
+        <v>Junier</v>
+      </c>
+      <c r="C33" t="str">
+        <v>Oliva</v>
+      </c>
+      <c r="D33">
+        <v>730295982</v>
+      </c>
+      <c r="E33" t="b">
+        <v>1</v>
+      </c>
+      <c r="F33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>pizer</v>
+      </c>
+      <c r="B34" t="str">
+        <v>Steve</v>
+      </c>
+      <c r="C34" t="str">
+        <v>Pizer</v>
+      </c>
+      <c r="D34">
+        <v>704208957</v>
+      </c>
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>plaisted</v>
+      </c>
+      <c r="B35" t="str">
+        <v>David</v>
+      </c>
+      <c r="C35" t="str">
+        <v>Plaisted</v>
+      </c>
+      <c r="D35">
+        <v>704213001</v>
+      </c>
+      <c r="E35" t="b">
+        <v>1</v>
+      </c>
+      <c r="F35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>porter</v>
+      </c>
+      <c r="B36" t="str">
+        <v>Donald</v>
+      </c>
+      <c r="C36" t="str">
+        <v>Porter</v>
+      </c>
+      <c r="D36">
+        <v>711757923</v>
+      </c>
+      <c r="E36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>pozefsky</v>
+      </c>
+      <c r="B37" t="str">
+        <v>Diane</v>
+      </c>
+      <c r="C37" t="str">
+        <v>Pozefsky</v>
+      </c>
+      <c r="D37">
+        <v>701569707</v>
+      </c>
+      <c r="E37" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>prins</v>
+      </c>
+      <c r="B38" t="str">
+        <v>Jan</v>
+      </c>
+      <c r="C38" t="str">
+        <v>Prins</v>
+      </c>
+      <c r="D38">
+        <v>704216581</v>
+      </c>
+      <c r="E38" t="b">
+        <v>1</v>
+      </c>
+      <c r="F38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>mreed</v>
+      </c>
+      <c r="B39" t="str">
+        <v>Mike</v>
+      </c>
+      <c r="C39" t="str">
+        <v>Reed</v>
+      </c>
+      <c r="D39">
+        <v>701628233</v>
+      </c>
+      <c r="E39" t="b">
+        <v>1</v>
+      </c>
+      <c r="F39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>reiter</v>
+      </c>
+      <c r="B40" t="str">
+        <v>Michael</v>
+      </c>
+      <c r="C40" t="str">
+        <v>Reiter</v>
+      </c>
+      <c r="D40">
+        <v>702350621</v>
+      </c>
+      <c r="E40" t="b">
+        <v>1</v>
+      </c>
+      <c r="F40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>Takoda</v>
+      </c>
+      <c r="B41" t="str">
+        <v>Takoda</v>
+      </c>
+      <c r="C41" t="str">
+        <v>Ren</v>
+      </c>
+      <c r="D41">
+        <v>730093699</v>
+      </c>
+      <c r="E41" t="b">
+        <v>1</v>
+      </c>
+      <c r="F41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>rosenman</v>
+      </c>
+      <c r="B42" t="str">
+        <v>Julian</v>
+      </c>
+      <c r="C42" t="str">
+        <v>Rosenman</v>
+      </c>
+      <c r="D42">
+        <v>704271584</v>
+      </c>
+      <c r="E42" t="b">
+        <v>1</v>
+      </c>
+      <c r="F42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>jsilva</v>
+      </c>
+      <c r="B43" t="str">
+        <v>Jorge</v>
+      </c>
+      <c r="C43" t="str">
+        <v>Silva</v>
+      </c>
+      <c r="D43">
+        <v>730139149</v>
+      </c>
+      <c r="E43" t="b">
+        <v>1</v>
+      </c>
+      <c r="F43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>montek</v>
+      </c>
+      <c r="B44" t="str">
+        <v>Montek</v>
+      </c>
+      <c r="C44" t="str">
+        <v>Singh</v>
+      </c>
+      <c r="D44">
+        <v>709856816</v>
+      </c>
+      <c r="E44" t="b">
+        <v>1</v>
+      </c>
+      <c r="F44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>smithfd</v>
+      </c>
+      <c r="B45" t="str">
+        <v>Don</v>
+      </c>
+      <c r="C45" t="str">
+        <v>Smith</v>
+      </c>
+      <c r="D45">
+        <v>701875776</v>
+      </c>
+      <c r="E45" t="b">
+        <v>1</v>
+      </c>
+      <c r="F45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
         <v>snoeyink</v>
       </c>
-      <c r="D12">
-        <v>111111111</v>
-      </c>
-      <c r="E12" t="b">
-        <v>1</v>
+      <c r="B46" t="str">
+        <v>Jack</v>
+      </c>
+      <c r="C46" t="str">
+        <v>Snoeyink</v>
+      </c>
+      <c r="D46">
+        <v>706390995</v>
+      </c>
+      <c r="E46" t="b">
+        <v>1</v>
+      </c>
+      <c r="F46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>stotts</v>
+      </c>
+      <c r="B47" t="str">
+        <v>David</v>
+      </c>
+      <c r="C47" t="str">
+        <v>Stotts</v>
+      </c>
+      <c r="D47">
+        <v>704225848</v>
+      </c>
+      <c r="E47" t="b">
+        <v>1</v>
+      </c>
+      <c r="F47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>csturton</v>
+      </c>
+      <c r="B48" t="str">
+        <v>Cynthia</v>
+      </c>
+      <c r="C48" t="str">
+        <v>Sturton</v>
+      </c>
+      <c r="D48">
+        <v>713811780</v>
+      </c>
+      <c r="E48" t="b">
+        <v>1</v>
+      </c>
+      <c r="F48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>styner</v>
+      </c>
+      <c r="B49" t="str">
+        <v>Martin</v>
+      </c>
+      <c r="C49" t="str">
+        <v>Styner</v>
+      </c>
+      <c r="D49">
+        <v>704313363</v>
+      </c>
+      <c r="E49" t="b">
+        <v>1</v>
+      </c>
+      <c r="F49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>taylorr</v>
+      </c>
+      <c r="B50" t="str">
+        <v>Russell</v>
+      </c>
+      <c r="C50" t="str">
+        <v>Taylor</v>
+      </c>
+      <c r="D50">
+        <v>702502169</v>
+      </c>
+      <c r="E50" t="b">
+        <v>1</v>
+      </c>
+      <c r="F50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>terrell</v>
+      </c>
+      <c r="B51" t="str">
+        <v>Jeff</v>
+      </c>
+      <c r="C51" t="str">
+        <v>Terrell</v>
+      </c>
+      <c r="D51">
+        <v>710985109</v>
+      </c>
+      <c r="E51" t="b">
+        <v>1</v>
+      </c>
+      <c r="F51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>whitton</v>
+      </c>
+      <c r="B52" t="str">
+        <v>Mary</v>
+      </c>
+      <c r="C52" t="str">
+        <v>Whitton</v>
+      </c>
+      <c r="D52">
+        <v>700599204</v>
+      </c>
+      <c r="E52" t="b">
+        <v>1</v>
+      </c>
+      <c r="F52" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H52"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Set up general structure of new forms (routes, view, controller, model). Also fixed formatting on student view.
</commit_message>
<xml_diff>
--- a/data/facultyTemp.xlsx
+++ b/data/facultyTemp.xlsx
@@ -429,7 +429,7 @@
         <v>sdfasdf</v>
       </c>
       <c r="H2">
-        <v>33</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3">
@@ -455,7 +455,7 @@
         <v>the</v>
       </c>
       <c r="H3">
-        <v>234</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4">
@@ -477,6 +477,12 @@
       <c r="F4" t="b">
         <v>0</v>
       </c>
+      <c r="G4" t="str">
+        <v>ron</v>
+      </c>
+      <c r="H4">
+        <v>33</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -497,6 +503,12 @@
       <c r="F5" t="b">
         <v>0</v>
       </c>
+      <c r="G5" t="str">
+        <v>anderson</v>
+      </c>
+      <c r="H5">
+        <v>33</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -521,7 +533,7 @@
         <v>Tasd</v>
       </c>
       <c r="H6">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7">
@@ -543,6 +555,12 @@
       <c r="F7" t="b">
         <v>0</v>
       </c>
+      <c r="G7" t="str">
+        <v>mbansal</v>
+      </c>
+      <c r="H7">
+        <v>33</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -563,6 +581,12 @@
       <c r="F8" t="b">
         <v>0</v>
       </c>
+      <c r="G8" t="str">
+        <v>aberg</v>
+      </c>
+      <c r="H8">
+        <v>33</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -583,6 +607,12 @@
       <c r="F9" t="b">
         <v>0</v>
       </c>
+      <c r="G9" t="str">
+        <v>tlberg</v>
+      </c>
+      <c r="H9">
+        <v>33</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -603,6 +633,12 @@
       <c r="F10" t="b">
         <v>0</v>
       </c>
+      <c r="G10" t="str">
+        <v>gb</v>
+      </c>
+      <c r="H10">
+        <v>33</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -623,6 +659,12 @@
       <c r="F11" t="b">
         <v>0</v>
       </c>
+      <c r="G11" t="str">
+        <v>dewan</v>
+      </c>
+      <c r="H11">
+        <v>33</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -643,6 +685,12 @@
       <c r="F12" t="b">
         <v>0</v>
       </c>
+      <c r="G12" t="str">
+        <v>psd</v>
+      </c>
+      <c r="H12">
+        <v>33</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -663,6 +711,12 @@
       <c r="F13" t="b">
         <v>0</v>
       </c>
+      <c r="G13" t="str">
+        <v>dunn</v>
+      </c>
+      <c r="H13">
+        <v>33</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -683,6 +737,12 @@
       <c r="F14" t="b">
         <v>0</v>
       </c>
+      <c r="G14" t="str">
+        <v>fern</v>
+      </c>
+      <c r="H14">
+        <v>33</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -703,6 +763,12 @@
       <c r="F15" t="b">
         <v>1</v>
       </c>
+      <c r="G15" t="str">
+        <v>Svflann</v>
+      </c>
+      <c r="H15">
+        <v>33</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -723,6 +789,12 @@
       <c r="F16" t="b">
         <v>0</v>
       </c>
+      <c r="G16" t="str">
+        <v>rjf</v>
+      </c>
+      <c r="H16">
+        <v>33</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -743,6 +815,12 @@
       <c r="F17" t="b">
         <v>0</v>
       </c>
+      <c r="G17" t="str">
+        <v>jmf</v>
+      </c>
+      <c r="H17">
+        <v>33</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -763,6 +841,12 @@
       <c r="F18" t="b">
         <v>0</v>
       </c>
+      <c r="G18" t="str">
+        <v>fuchs</v>
+      </c>
+      <c r="H18">
+        <v>33</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -783,6 +867,12 @@
       <c r="F19" t="b">
         <v>0</v>
       </c>
+      <c r="G19" t="str">
+        <v>jeffay</v>
+      </c>
+      <c r="H19">
+        <v>33</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -803,6 +893,12 @@
       <c r="F20" t="b">
         <v>0</v>
       </c>
+      <c r="G20" t="str">
+        <v>kris</v>
+      </c>
+      <c r="H20">
+        <v>33</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -823,6 +919,12 @@
       <c r="F21" t="b">
         <v>0</v>
       </c>
+      <c r="G21" t="str">
+        <v>nicholas</v>
+      </c>
+      <c r="H21">
+        <v>33</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -843,6 +945,12 @@
       <c r="F22" t="b">
         <v>0</v>
       </c>
+      <c r="G22" t="str">
+        <v>jasleen</v>
+      </c>
+      <c r="H22">
+        <v>33</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -863,6 +971,12 @@
       <c r="F23" t="b">
         <v>0</v>
       </c>
+      <c r="G23" t="str">
+        <v>ashokk</v>
+      </c>
+      <c r="H23">
+        <v>33</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -883,6 +997,12 @@
       <c r="F24" t="b">
         <v>0</v>
       </c>
+      <c r="G24" t="str">
+        <v>lin</v>
+      </c>
+      <c r="H24">
+        <v>33</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -903,6 +1023,12 @@
       <c r="F25" t="b">
         <v>0</v>
       </c>
+      <c r="G25" t="str">
+        <v>jmajikes</v>
+      </c>
+      <c r="H25">
+        <v>33</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -923,6 +1049,12 @@
       <c r="F26" t="b">
         <v>0</v>
       </c>
+      <c r="G26" t="str">
+        <v>dm</v>
+      </c>
+      <c r="H26">
+        <v>33</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
@@ -943,6 +1075,12 @@
       <c r="F27" t="b">
         <v>0</v>
       </c>
+      <c r="G27" t="str">
+        <v>kmp</v>
+      </c>
+      <c r="H27">
+        <v>33</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
@@ -963,6 +1101,12 @@
       <c r="F28" t="b">
         <v>0</v>
       </c>
+      <c r="G28" t="str">
+        <v>mcmillan</v>
+      </c>
+      <c r="H28">
+        <v>33</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
@@ -983,6 +1127,12 @@
       <c r="F29" t="b">
         <v>0</v>
       </c>
+      <c r="G29" t="str">
+        <v>fabian</v>
+      </c>
+      <c r="H29">
+        <v>33</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
@@ -1003,6 +1153,12 @@
       <c r="F30" t="b">
         <v>0</v>
       </c>
+      <c r="G30" t="str">
+        <v>mn</v>
+      </c>
+      <c r="H30">
+        <v>33</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
@@ -1023,6 +1179,12 @@
       <c r="F31" t="b">
         <v>0</v>
       </c>
+      <c r="G31" t="str">
+        <v>nirjon</v>
+      </c>
+      <c r="H31">
+        <v>33</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
@@ -1043,6 +1205,12 @@
       <c r="F32" t="b">
         <v>0</v>
       </c>
+      <c r="G32" t="str">
+        <v>ipek</v>
+      </c>
+      <c r="H32">
+        <v>33</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
@@ -1063,6 +1231,12 @@
       <c r="F33" t="b">
         <v>0</v>
       </c>
+      <c r="G33" t="str">
+        <v>joliva</v>
+      </c>
+      <c r="H33">
+        <v>33</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
@@ -1083,6 +1257,12 @@
       <c r="F34" t="b">
         <v>0</v>
       </c>
+      <c r="G34" t="str">
+        <v>pizer</v>
+      </c>
+      <c r="H34">
+        <v>33</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
@@ -1103,6 +1283,12 @@
       <c r="F35" t="b">
         <v>0</v>
       </c>
+      <c r="G35" t="str">
+        <v>plaisted</v>
+      </c>
+      <c r="H35">
+        <v>33</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
@@ -1123,6 +1309,12 @@
       <c r="F36" t="b">
         <v>0</v>
       </c>
+      <c r="G36" t="str">
+        <v>porter</v>
+      </c>
+      <c r="H36">
+        <v>33</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
@@ -1141,7 +1333,13 @@
         <v>1</v>
       </c>
       <c r="F37" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G37" t="str">
+        <v>pozefsky</v>
+      </c>
+      <c r="H37">
+        <v>33</v>
       </c>
     </row>
     <row r="38">
@@ -1163,6 +1361,12 @@
       <c r="F38" t="b">
         <v>0</v>
       </c>
+      <c r="G38" t="str">
+        <v>prins</v>
+      </c>
+      <c r="H38">
+        <v>33</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
@@ -1183,6 +1387,12 @@
       <c r="F39" t="b">
         <v>0</v>
       </c>
+      <c r="G39" t="str">
+        <v>mreed</v>
+      </c>
+      <c r="H39">
+        <v>33</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
@@ -1203,6 +1413,12 @@
       <c r="F40" t="b">
         <v>0</v>
       </c>
+      <c r="G40" t="str">
+        <v>reiter</v>
+      </c>
+      <c r="H40">
+        <v>33</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
@@ -1223,6 +1439,12 @@
       <c r="F41" t="b">
         <v>1</v>
       </c>
+      <c r="G41" t="str">
+        <v>Takoda</v>
+      </c>
+      <c r="H41">
+        <v>33</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
@@ -1243,6 +1465,12 @@
       <c r="F42" t="b">
         <v>0</v>
       </c>
+      <c r="G42" t="str">
+        <v>rosenman</v>
+      </c>
+      <c r="H42">
+        <v>33</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
@@ -1263,6 +1491,12 @@
       <c r="F43" t="b">
         <v>0</v>
       </c>
+      <c r="G43" t="str">
+        <v>jsilva</v>
+      </c>
+      <c r="H43">
+        <v>33</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
@@ -1283,6 +1517,12 @@
       <c r="F44" t="b">
         <v>0</v>
       </c>
+      <c r="G44" t="str">
+        <v>montek</v>
+      </c>
+      <c r="H44">
+        <v>33</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
@@ -1303,6 +1543,12 @@
       <c r="F45" t="b">
         <v>0</v>
       </c>
+      <c r="G45" t="str">
+        <v>smithfd</v>
+      </c>
+      <c r="H45">
+        <v>33</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
@@ -1323,6 +1569,12 @@
       <c r="F46" t="b">
         <v>0</v>
       </c>
+      <c r="G46" t="str">
+        <v>snoeyink</v>
+      </c>
+      <c r="H46">
+        <v>33</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
@@ -1343,6 +1595,12 @@
       <c r="F47" t="b">
         <v>0</v>
       </c>
+      <c r="G47" t="str">
+        <v>stotts</v>
+      </c>
+      <c r="H47">
+        <v>33</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
@@ -1363,6 +1621,12 @@
       <c r="F48" t="b">
         <v>0</v>
       </c>
+      <c r="G48" t="str">
+        <v>csturton</v>
+      </c>
+      <c r="H48">
+        <v>33</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
@@ -1383,6 +1647,12 @@
       <c r="F49" t="b">
         <v>0</v>
       </c>
+      <c r="G49" t="str">
+        <v>styner</v>
+      </c>
+      <c r="H49">
+        <v>33</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
@@ -1403,6 +1673,12 @@
       <c r="F50" t="b">
         <v>0</v>
       </c>
+      <c r="G50" t="str">
+        <v>taylorr</v>
+      </c>
+      <c r="H50">
+        <v>33</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
@@ -1423,6 +1699,12 @@
       <c r="F51" t="b">
         <v>0</v>
       </c>
+      <c r="G51" t="str">
+        <v>terrell</v>
+      </c>
+      <c r="H51">
+        <v>33</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
@@ -1442,6 +1724,12 @@
       </c>
       <c r="F52" t="b">
         <v>0</v>
+      </c>
+      <c r="G52" t="str">
+        <v>whitton</v>
+      </c>
+      <c r="H52">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>